<commit_message>
add summary bug report
</commit_message>
<xml_diff>
--- a/Testing/Reports/Car-Bug-Reports.xlsx
+++ b/Testing/Reports/Car-Bug-Reports.xlsx
@@ -9,23 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8796" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8796" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="add_car_bug_report" sheetId="1" r:id="rId1"/>
     <sheet name="update_car_bug_report" sheetId="2" r:id="rId2"/>
     <sheet name="Login" sheetId="3" r:id="rId3"/>
     <sheet name="Registration" sheetId="5" r:id="rId4"/>
+    <sheet name="SummaryReport" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">update_car_bug_report!$A$1:$R$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="138">
   <si>
     <t>ID</t>
   </si>
@@ -549,6 +550,45 @@
   <si>
     <t>There is no Home button is exist in the update car page as mentioned in SRS</t>
   </si>
+  <si>
+    <t>Related page</t>
+  </si>
+  <si>
+    <t>Number of Bugs</t>
+  </si>
+  <si>
+    <t>Test cases Numbers</t>
+  </si>
+  <si>
+    <t>Add Car</t>
+  </si>
+  <si>
+    <t>Update Car</t>
+  </si>
+  <si>
+    <t>User Home page</t>
+  </si>
+  <si>
+    <t>Admin home page</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>All Pages</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Tests passed</t>
+  </si>
 </sst>
 </file>
 
@@ -557,7 +597,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -669,8 +709,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -706,8 +753,14 @@
         <bgColor rgb="FFB3CEFA"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4285F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -795,12 +848,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -919,6 +987,19 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -935,6 +1016,901 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-D98B-4275-B082-204DB33B42A7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-D98B-4275-B082-204DB33B42A7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-D98B-4275-B082-204DB33B42A7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-D98B-4275-B082-204DB33B42A7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>SummaryReport!$A$12:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Passed</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Failed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SummaryReport!$B$12:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D98B-4275-B082-204DB33B42A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1140,7 +2116,7 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
@@ -28225,8 +29201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
@@ -30238,4 +31214,166 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="46">
+        <v>2</v>
+      </c>
+      <c r="C2" s="46">
+        <v>12</v>
+      </c>
+      <c r="D2" s="46">
+        <f>C2-B2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="46">
+        <v>4</v>
+      </c>
+      <c r="C3" s="46">
+        <v>23</v>
+      </c>
+      <c r="D3" s="46">
+        <f t="shared" ref="D3:D7" si="0">C3-B3</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="46">
+        <v>0</v>
+      </c>
+      <c r="C4" s="46">
+        <v>3</v>
+      </c>
+      <c r="D4" s="46">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="46">
+        <v>0</v>
+      </c>
+      <c r="C5" s="46">
+        <v>5</v>
+      </c>
+      <c r="D5" s="46">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="46">
+        <v>4</v>
+      </c>
+      <c r="C6" s="46">
+        <v>18</v>
+      </c>
+      <c r="D6" s="46">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="46">
+        <v>1</v>
+      </c>
+      <c r="C7" s="46">
+        <v>14</v>
+      </c>
+      <c r="D7" s="46">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="46">
+        <f>SUM(B2:B7)</f>
+        <v>11</v>
+      </c>
+      <c r="C8" s="46">
+        <f>SUM(C2:C7)</f>
+        <v>75</v>
+      </c>
+      <c r="D8" s="46">
+        <f>SUM(D2:D7)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="48">
+        <f>D8</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="48">
+        <f>B8</f>
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>